<commit_message>
Added Connectors across multiple divs
</commit_message>
<xml_diff>
--- a/Reference Links.xlsx
+++ b/Reference Links.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Agenda" sheetId="1" r:id="rId1"/>
+    <sheet name="Work Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Tasks</t>
   </si>
@@ -61,6 +62,93 @@
   </si>
   <si>
     <t>Create State Diagram</t>
+  </si>
+  <si>
+    <t>Add connector between 2 divs</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>March 28th - March 31st</t>
+  </si>
+  <si>
+    <t>Analysed class diagram, sequence diagram</t>
+  </si>
+  <si>
+    <t>learned more about go js api</t>
+  </si>
+  <si>
+    <t>April 2nd - April 7th</t>
+  </si>
+  <si>
+    <t>Analysed State Chart</t>
+  </si>
+  <si>
+    <t>April 9th - April 14th</t>
+  </si>
+  <si>
+    <t>Drag and Drop</t>
+  </si>
+  <si>
+    <t>Realized the elements are not permitted to be dragged and cause error when placed next to each other</t>
+  </si>
+  <si>
+    <t>Assessed another way to create the library</t>
+  </si>
+  <si>
+    <t>Designed classes for class diagram</t>
+  </si>
+  <si>
+    <t>Divided a div into 3 parts for name,function,variable</t>
+  </si>
+  <si>
+    <t>positioning</t>
+  </si>
+  <si>
+    <t>Added drag functionality for classes</t>
+  </si>
+  <si>
+    <t>Allowing multiple divs across a page to be draggable.</t>
+  </si>
+  <si>
+    <t>Implemented drag without any library and using pure javascript to prevent copyright.</t>
+  </si>
+  <si>
+    <t>April 25th</t>
+  </si>
+  <si>
+    <t>Creating Connectors</t>
+  </si>
+  <si>
+    <t>Analysed how to do task and searched for approximate references</t>
+  </si>
+  <si>
+    <t>That there is a svg tag in html</t>
+  </si>
+  <si>
+    <t>Connect two divs</t>
+  </si>
+  <si>
+    <t>Get position of the element and update everytime the person drags them so the connector lines stay intact</t>
+  </si>
+  <si>
+    <t>That we can access the exact position of any tag in html using JavaScript</t>
+  </si>
+  <si>
+    <t>April 26th onwards</t>
+  </si>
+  <si>
+    <t>Using previous tasks, create a class diagram, sequence diagram and state diagram</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Sub-Task</t>
+  </si>
+  <si>
+    <t>Learning</t>
   </si>
 </sst>
 </file>
@@ -104,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,11 +206,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -142,18 +243,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -168,12 +257,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:D18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B1:D18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:D19" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B1:D19"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Sr No." dataDxfId="4"/>
-    <tableColumn id="2" name="Tasks" dataDxfId="3"/>
-    <tableColumn id="3" name="Recommended Links" dataDxfId="2"/>
+    <tableColumn id="1" name="Sr No." dataDxfId="2"/>
+    <tableColumn id="2" name="Tasks" dataDxfId="1"/>
+    <tableColumn id="3" name="Recommended Links" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -442,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D18"/>
+  <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,26 +566,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -504,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -512,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -520,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -528,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -536,13 +625,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>9</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -582,6 +674,11 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -591,4 +688,141 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>